<commit_message>
test gemma 3 embed
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keven\Desktop\倪宇健\NYU\大三\DS 301\Project\NYU-Policy-LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E136003F-8081-4FBB-A010-A19E15EB46D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B508A037-D065-49AA-99FD-BC06F86F0B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -175,9 +175,6 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -479,9 +476,9 @@
     <col min="11" max="11" width="18.06640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="19.06640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.265625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.19921875" customWidth="1"/>
-    <col min="15" max="15" width="18.19921875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.86328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.86328125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.19921875" customWidth="1"/>
+    <col min="16" max="16" width="18.19921875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
@@ -523,14 +520,14 @@
       <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
@@ -573,12 +570,14 @@
       <c r="M2" s="3">
         <v>0.47370000000000001</v>
       </c>
-      <c r="N2" s="6"/>
+      <c r="N2" s="4">
+        <v>0.26319999999999999</v>
+      </c>
       <c r="O2" s="3">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="P2" s="3">
         <v>0.85</v>
-      </c>
-      <c r="P2" s="4">
-        <v>0.26319999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.5">
@@ -621,12 +620,14 @@
       <c r="M3" s="3">
         <v>0.05</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="4">
+        <v>0.25</v>
+      </c>
       <c r="O3" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="P3" s="3">
         <v>1</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.5">
@@ -669,12 +670,14 @@
       <c r="M4" s="3">
         <v>0.4</v>
       </c>
-      <c r="N4" s="6"/>
+      <c r="N4" s="4">
+        <v>0.4</v>
+      </c>
       <c r="O4" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P4" s="3">
         <v>0.95</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.5">
@@ -717,12 +720,14 @@
       <c r="M5" s="4">
         <v>0.32500000000000001</v>
       </c>
-      <c r="N5" s="6"/>
+      <c r="N5" s="4">
+        <v>0.375</v>
+      </c>
       <c r="O5" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="P5" s="3">
         <v>0.8</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0.375</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.5">
@@ -765,12 +770,14 @@
       <c r="M6" s="3">
         <v>0.7</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="3">
+        <v>0.7</v>
+      </c>
       <c r="O6" s="3">
         <v>0.75</v>
       </c>
       <c r="P6" s="3">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.5">
@@ -813,12 +820,14 @@
       <c r="M7" s="3">
         <v>0.3</v>
       </c>
-      <c r="N7" s="6"/>
+      <c r="N7" s="3">
+        <v>0.45</v>
+      </c>
       <c r="O7" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P7" s="3">
         <v>0.85</v>
-      </c>
-      <c r="P7" s="3">
-        <v>0.45</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.5">
@@ -861,12 +870,14 @@
       <c r="M8" s="3">
         <v>0.37</v>
       </c>
-      <c r="N8" s="6"/>
+      <c r="N8" s="4">
+        <v>0.40600000000000003</v>
+      </c>
       <c r="O8" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="P8" s="3">
         <v>0.87</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0.40600000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add llama fine tune
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keven\Desktop\倪宇健\NYU\大三\DS 301\Project\NYU-Policy-LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B508A037-D065-49AA-99FD-BC06F86F0B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E73181-1640-4D2D-B757-B94C770B131F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Gemini 2.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +112,10 @@
   </si>
   <si>
     <t>Mistral Fine-tuned</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Llamma3 Fine-tunded</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -456,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -471,18 +475,19 @@
     <col min="5" max="5" width="13.46484375" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.46484375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.46484375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.265625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.06640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.06640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.265625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="23.86328125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.19921875" customWidth="1"/>
-    <col min="16" max="16" width="18.19921875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.06640625" style="1"/>
+    <col min="8" max="8" width="23.86328125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="16.46484375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.06640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.06640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="23.86328125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.19921875" customWidth="1"/>
+    <col min="17" max="17" width="18.19921875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -503,34 +508,37 @@
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -553,34 +561,37 @@
         <v>0.35</v>
       </c>
       <c r="H2" s="3">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="I2" s="3">
         <v>0.45</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>0.42</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>0.36840000000000001</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>0.5</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>0.85</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>0.47370000000000001</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>0.26319999999999999</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="3">
         <v>0.57899999999999996</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>0.85</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -603,34 +614,37 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="H3" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="4">
         <v>0.75</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.3</v>
       </c>
       <c r="J3" s="4">
         <v>0.3</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L3" s="3">
         <v>0.65</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>0.95</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>0.05</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <v>0.25</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>0.6</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -653,34 +667,37 @@
         <v>0.5</v>
       </c>
       <c r="H4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="I4" s="3">
         <v>0.9</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>0.2</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>0.6</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>0.9</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>0.4</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <v>0.4</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>0.75</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -703,34 +720,37 @@
         <v>0.375</v>
       </c>
       <c r="H5" s="4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="I5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="J5" s="4">
         <v>0.5</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>0.375</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>0.65</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <v>0.72499999999999998</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>0.32500000000000001</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>0.375</v>
       </c>
-      <c r="O5" s="3">
-        <v>0.7</v>
-      </c>
       <c r="P5" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="Q5" s="3">
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -753,34 +773,37 @@
         <v>0.6</v>
       </c>
       <c r="H6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="I6" s="3">
         <v>0.65</v>
       </c>
-      <c r="I6" s="3">
-        <v>0.7</v>
-      </c>
       <c r="J6" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K6" s="3">
         <v>0.5</v>
       </c>
-      <c r="K6" s="3">
-        <v>0.7</v>
-      </c>
       <c r="L6" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="M6" s="3">
         <v>0.95</v>
       </c>
-      <c r="M6" s="3">
-        <v>0.7</v>
-      </c>
       <c r="N6" s="3">
         <v>0.7</v>
       </c>
       <c r="O6" s="3">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="P6" s="3">
         <v>0.75</v>
       </c>
+      <c r="Q6" s="3">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -803,34 +826,37 @@
         <v>0.5</v>
       </c>
       <c r="H7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="3">
         <v>0.85</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>0.3</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>0.2</v>
       </c>
-      <c r="K7" s="3">
-        <v>0.7</v>
-      </c>
       <c r="L7" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="M7" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="3">
         <v>0.3</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>0.45</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -853,30 +879,33 @@
         <v>0.48</v>
       </c>
       <c r="H8" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="3">
         <v>0.72</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>0.46</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>0.32</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>0.63329999999999997</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>0.82</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="3">
         <v>0.37</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
         <v>0.40600000000000003</v>
       </c>
-      <c r="O8" s="3">
+      <c r="P8" s="3">
         <v>0.65</v>
       </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="3">
         <v>0.87</v>
       </c>
     </row>

</xml_diff>